<commit_message>
to input correct format
</commit_message>
<xml_diff>
--- a/documents/WBS.xlsx
+++ b/documents/WBS.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b8543b8d03b7b4a0/Projects/asd/BankingSystem/documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MUM\MUM_Course\WAP_09282020\Assignment\bankproj\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="114_{16404DF6-EFAA-7C40-99E5-252F5E0B841E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{61818ED9-CB94-4E54-B2D0-123B86C9965B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19080" xr2:uid="{26B21BE0-F582-4599-956B-3993E3646063}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{26B21BE0-F582-4599-956B-3993E3646063}"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="1" r:id="rId1"/>
     <sheet name="Data Test" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="65">
   <si>
     <t>WBS - Team 6</t>
   </si>
@@ -52,16 +52,145 @@
     <t>PIC</t>
   </si>
   <si>
+    <t>Duc Phuoc Doan</t>
+  </si>
+  <si>
+    <t>Duy Thai Nguyen</t>
+  </si>
+  <si>
+    <t>Personal Account -&gt; Deposit/Withdraw/Calculate Interest</t>
+  </si>
+  <si>
+    <t>Create Credit Card -&gt; Deposit/Charge Account</t>
+  </si>
+  <si>
+    <t>Credit Interest: interest and Payment</t>
+  </si>
+  <si>
+    <t>Company Account -&gt; Calculate Interest</t>
+  </si>
+  <si>
+    <t>Integration and Testing</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Integrate the whole system and do testing</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Biniam Tsehaye Arefaine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No. </t>
+  </si>
+  <si>
+    <t>Checking/Saving</t>
+  </si>
+  <si>
+    <t>AccountNo</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Checking </t>
+  </si>
+  <si>
+    <t xml:space="preserve">N 1st </t>
+  </si>
+  <si>
+    <t>Fairfield</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>Saving</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N 2nd </t>
+  </si>
+  <si>
+    <t>N 3rd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N 4th </t>
+  </si>
+  <si>
+    <t>Personal Account</t>
+  </si>
+  <si>
+    <t>C001-0001</t>
+  </si>
+  <si>
+    <t>C001-0002</t>
+  </si>
+  <si>
+    <t>C001-0003</t>
+  </si>
+  <si>
+    <t>C001-0004</t>
+  </si>
+  <si>
+    <t>P001-1001</t>
+  </si>
+  <si>
+    <t>P001-1002</t>
+  </si>
+  <si>
+    <t>P001-1003</t>
+  </si>
+  <si>
+    <t>P001-1004</t>
+  </si>
+  <si>
+    <t>Deposit</t>
+  </si>
+  <si>
+    <t>Interest</t>
+  </si>
+  <si>
+    <t>Withdraw</t>
+  </si>
+  <si>
+    <t>Num</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>1960-01-01</t>
+  </si>
+  <si>
     <t>Status</t>
   </si>
   <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>In reviewing the all deliverables</t>
+  </si>
+  <si>
+    <t>Yohannes Teweldeberhan.</t>
+  </si>
+  <si>
     <t>Project framework: common framework for 2 application, then put in Github</t>
-  </si>
-  <si>
-    <t>Duc Phuoc Doan</t>
-  </si>
-  <si>
-    <t>Done</t>
   </si>
   <si>
     <t xml:space="preserve">Class Diagram </t>
@@ -72,13 +201,54 @@
 - Maintain during changes in implementation</t>
   </si>
   <si>
-    <t>Duy Thai Nguyen</t>
-  </si>
-  <si>
-    <t>Personal Account -&gt; Deposit/Withdraw/Calculate Interest</t>
-  </si>
-  <si>
-    <t>Full flow from DB to UI. Strategy Pattern and Observer pattern these functions: 
+    <t>Report for the part 1, Bank Statement
+- Review Class diagram
+- Implementation
+- Sequence Diagram</t>
+  </si>
+  <si>
+    <t>Report for the part 2, Billing report
+- Review Class diagram
+- Implementation
+- Sequence Diagram</t>
+  </si>
+  <si>
+    <t>Generate Report of Banking application</t>
+  </si>
+  <si>
+    <t>Full flow from DB to UI,  and Observer pattern:
+- Create CreditCard
+- Deposit and Charge
+For each feature, we do below tasks: 
+- Review Class diagram
+- Implementation
+- Sequence Diagram</t>
+  </si>
+  <si>
+    <t>Generate Billing report of Credit Card application</t>
+  </si>
+  <si>
+    <t>Full flow from DB to UI, Strategy and Observer pattern (mail inform):
+- Interest
+- Min Payment
+For each, do below tasks: 
+- Review Class diagram
+- Implementation
+- Sequence Diagram</t>
+  </si>
+  <si>
+    <t>ndt.rachkien@gmail.com</t>
+  </si>
+  <si>
+    <t>- Create project structure, framework for starting the implementation
+- Update framework during implementation
+- Apply Singleton pattern for AcountDAO</t>
+  </si>
+  <si>
+    <t>Tesfai Habtai Samuel</t>
+  </si>
+  <si>
+    <t>To implement full flow from DB to UI, apply Strategy Pattern and Observer pattern these functions: 
 - Create Personal Account
 - Deposit and Withdraw
 - Calculate interests
@@ -88,10 +258,7 @@
 - Sequence Diagram</t>
   </si>
   <si>
-    <t>Company Account -&gt; Calculate Interest</t>
-  </si>
-  <si>
-    <t>Full flow from DB to UI. Strategy Pattern and Observer pattern these functions: 
+    <t>To implement full flow from DB to UI, apply Strategy Pattern and Observer pattern these functions: 
 - Create Company Account
 - Deposit and Withdraw
 - Calculate interests
@@ -99,201 +266,6 @@
 - Review Class diagram
 - Implementation
 - Sequence Diagram</t>
-  </si>
-  <si>
-    <t>Generate Billing report of Credit Card application</t>
-  </si>
-  <si>
-    <t>Report for the part 2, Billing report
-- Review Class diagram
-- Implementation
-- Apply Strategy pattern</t>
-  </si>
-  <si>
-    <t>Generate Report of Banking application</t>
-  </si>
-  <si>
-    <t>Report for the part 1, Bank Statement
-- Review Class diagram
-- Implementation
-- Sequence Diagram</t>
-  </si>
-  <si>
-    <t>Yohannes Teweldeberhan.</t>
-  </si>
-  <si>
-    <t>Report for the part 2, Billing report
-- Review Class diagram
-- Sequence Diagram</t>
-  </si>
-  <si>
-    <t>Create Credit Card -&gt; Deposit/Charge Account</t>
-  </si>
-  <si>
-    <t>Full flow from DB to UI,  and Observer pattern:
-- Create CreditCard
-- Deposit and Charge
-For each feature, we do below tasks: 
-- Review Class diagram
-- Implementation
-- Sequence Diagram</t>
-  </si>
-  <si>
-    <t>Biniam Tsehaye Arefaine</t>
-  </si>
-  <si>
-    <t>Credit Interest: interest and Payment</t>
-  </si>
-  <si>
-    <t>Full flow from DB to UI, Strategy and Observer pattern (mail inform):
-- Interest
-- Min Payment
-For each, do below tasks: 
-- Review Class diagram
-- Implementation
-- Sequence Diagram</t>
-  </si>
-  <si>
-    <t>Tesfai Habtai Samuel
-Yohannes Teweldeberhan.</t>
-  </si>
-  <si>
-    <t>Integration and Testing</t>
-  </si>
-  <si>
-    <t>Integrate the whole system and do testing</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>In reviewing the all deliverables</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No. </t>
-  </si>
-  <si>
-    <t>Checking/Saving</t>
-  </si>
-  <si>
-    <t>AccountNo</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Street</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>Zip</t>
-  </si>
-  <si>
-    <t>Num</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Deposit</t>
-  </si>
-  <si>
-    <t>Withdraw</t>
-  </si>
-  <si>
-    <t>Interest</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Checking </t>
-  </si>
-  <si>
-    <t>C001-0001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N 1st </t>
-  </si>
-  <si>
-    <t>Fairfield</t>
-  </si>
-  <si>
-    <t>IA</t>
-  </si>
-  <si>
-    <t>C001@gmail.com</t>
-  </si>
-  <si>
-    <t>C001-0002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N 2nd </t>
-  </si>
-  <si>
-    <t>C002@gmail.com</t>
-  </si>
-  <si>
-    <t>Saving</t>
-  </si>
-  <si>
-    <t>C001-0003</t>
-  </si>
-  <si>
-    <t>N 3rd</t>
-  </si>
-  <si>
-    <t>C003@gmail.com</t>
-  </si>
-  <si>
-    <t>C001-0004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N 4th </t>
-  </si>
-  <si>
-    <t>C004@gmail.com</t>
-  </si>
-  <si>
-    <t>Personal Account</t>
-  </si>
-  <si>
-    <t>P001-1001</t>
-  </si>
-  <si>
-    <t>1960-01-01</t>
-  </si>
-  <si>
-    <t>P001@gmail.com</t>
-  </si>
-  <si>
-    <t>P001-1002</t>
-  </si>
-  <si>
-    <t>P002@gmail.com</t>
-  </si>
-  <si>
-    <t>P001-1003</t>
-  </si>
-  <si>
-    <t>P003@gmail.com</t>
-  </si>
-  <si>
-    <t>P001-1004</t>
-  </si>
-  <si>
-    <t>P004@gmail.com</t>
-  </si>
-  <si>
-    <t>- Create project structure, framework for starting the implementation
-- Update framework during implementation
-- Apply Singleton pattern for database connector
-- Apply Composite pattern for Customer has multiple credit card</t>
   </si>
 </sst>
 </file>
@@ -437,7 +409,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -484,12 +456,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -507,6 +473,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -823,32 +792,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B79BA6-5186-4886-A71A-73B352D628AD}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="6"/>
-    <col min="2" max="2" width="38.5" style="18" customWidth="1"/>
-    <col min="3" max="3" width="55.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="6"/>
+    <col min="2" max="2" width="38.5703125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="55.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="31" style="1" customWidth="1"/>
-    <col min="5" max="5" width="31.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1640625" style="1"/>
+    <col min="5" max="5" width="31.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
-    </row>
-    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -862,177 +831,160 @@
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="144" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="144" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>20</v>
+        <v>54</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>50</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="19" t="s">
-        <v>16</v>
+      <c r="B9" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>20</v>
+        <v>57</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>15</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>24</v>
+        <v>59</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>62</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>27</v>
+        <v>11</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <v>10</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1049,88 +1001,88 @@
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" customWidth="1"/>
-    <col min="4" max="4" width="12.5" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" customWidth="1"/>
-    <col min="9" max="9" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25" customWidth="1"/>
-    <col min="13" max="13" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5" customWidth="1"/>
-    <col min="17" max="17" width="11.5" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="J1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="M1" s="10" t="s">
         <v>43</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="P1" s="13" t="s">
         <v>45</v>
       </c>
       <c r="Q1" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="7" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="H2" s="7">
         <v>52557</v>
@@ -1139,7 +1091,7 @@
         <v>5</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="L2" s="7">
         <v>10000</v>
@@ -1163,25 +1115,25 @@
         <v>4677.75</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="7" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="H3" s="7">
         <v>52557</v>
@@ -1190,7 +1142,7 @@
         <v>5</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="L3" s="7">
         <v>400</v>
@@ -1214,25 +1166,25 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="H4" s="7">
         <v>52557</v>
@@ -1241,7 +1193,7 @@
         <v>5</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L4" s="7">
         <v>20000</v>
@@ -1262,25 +1214,25 @@
         <v>22848</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="H5" s="7">
         <v>52557</v>
@@ -1289,7 +1241,7 @@
         <v>5</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L5" s="7">
         <v>500</v>
@@ -1310,19 +1262,19 @@
         <v>475.99999999999994</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="27"/>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="25"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
       <c r="N6" s="14"/>
@@ -1332,34 +1284,34 @@
       </c>
       <c r="Q6" s="14"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="H7" s="7">
         <v>52557</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="L7" s="7">
         <v>1000</v>
@@ -1383,34 +1335,34 @@
         <v>309.375</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="H8" s="7">
         <v>52557</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="L8" s="7">
         <v>40</v>
@@ -1434,34 +1386,34 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="H9" s="7">
         <v>52557</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="L9" s="7">
         <v>200</v>
@@ -1482,34 +1434,34 @@
         <v>115.19999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="H10" s="7">
         <v>52557</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="L10" s="7">
         <v>50</v>
@@ -1537,17 +1489,15 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" xr:uid="{3AED293F-EDD4-45C0-B35A-3CD236E0504D}"/>
-    <hyperlink ref="J3:J5" r:id="rId2" display="p001@gmail.com" xr:uid="{119C8857-D6B3-4877-85A0-4D0A5B429797}"/>
-    <hyperlink ref="J3" r:id="rId3" xr:uid="{65A9622B-F209-4E02-AFCD-5DC53F52F4D1}"/>
-    <hyperlink ref="J4" r:id="rId4" xr:uid="{65738428-C28E-435C-9BDF-A05DC266A3CF}"/>
-    <hyperlink ref="J5" r:id="rId5" xr:uid="{46E58D43-0225-40D4-AEC6-B44748BF00F0}"/>
-    <hyperlink ref="J7" r:id="rId6" xr:uid="{B29A8868-E247-4859-9019-CC3029C6F46E}"/>
-    <hyperlink ref="J8:J10" r:id="rId7" display="p001@gmail.com" xr:uid="{F4D24BDA-0C8C-4D92-9772-334B4F9B3DDD}"/>
-    <hyperlink ref="J8" r:id="rId8" xr:uid="{F9989DB6-81D6-4AF8-B460-4A928A3961B3}"/>
-    <hyperlink ref="J9" r:id="rId9" xr:uid="{0C363BFA-5E2D-4C60-8AEA-AE359776D9F9}"/>
-    <hyperlink ref="J10" r:id="rId10" xr:uid="{99F54E54-911A-43EE-B91D-4A8AC0BE4BBE}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{F2566113-747E-4DF1-ACC4-593C0C9335E0}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{CD348B69-4DFF-4759-A444-150E87CDD475}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{121C2EC9-A690-40D9-8E4F-515A8B27DB3E}"/>
+    <hyperlink ref="J7" r:id="rId5" xr:uid="{AC7738E5-79F4-4093-82FE-919A1AE4ED8D}"/>
+    <hyperlink ref="J8" r:id="rId6" xr:uid="{89DF4181-B685-4A5B-8469-506F2D6A2FA2}"/>
+    <hyperlink ref="J9" r:id="rId7" xr:uid="{FA5F37EA-46CB-43BC-B796-1C1F2FCF4558}"/>
+    <hyperlink ref="J10" r:id="rId8" xr:uid="{D7B5FAAF-63F4-486D-BD76-58B30B703F7E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>